<commit_message>
Added some error handling fixes
</commit_message>
<xml_diff>
--- a/res/Inventory.xlsx
+++ b/res/Inventory.xlsx
@@ -1300,14 +1300,18 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>GERMAN REMEDIES</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="n">
-        <v>898</v>
-      </c>
-      <c r="D33" s="12" t="n">
-        <v>44736</v>
+          <t>2026</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>898</t>
+        </is>
+      </c>
+      <c r="D33" s="12" t="inlineStr">
+        <is>
+          <t>23-06-2023</t>
+        </is>
       </c>
       <c r="E33" s="3" t="n">
         <v>83</v>

</xml_diff>